<commit_message>
updates to conc calculations, new HBEF data, recalculated FWMC, and created new MARSable df.
</commit_message>
<xml_diff>
--- a/data/JMHnewMungedDat/00_WatershedDataNotes.xlsx
+++ b/data/JMHnewMungedDat/00_WatershedDataNotes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hood.211/Dropbox/JMH_dropbox/stephanson2/projects/6_Research/IrenasPaper/bgc_meta/data/NewDataFromIrena20210130/New MAR Data/Raw Data Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hood.211/Dropbox/JMH_dropbox/stephanson2/projects/6_Research/IrenasPaper/bgc_meta/data/JMHnewMungedDat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10D9267-4581-2640-A412-F16884D7B3A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BEF8D0-E081-384A-92EC-3F38AD68A883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{BC43E26C-2443-B84E-92D9-98FD3EC23313}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{BC43E26C-2443-B84E-92D9-98FD3EC23313}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="96">
   <si>
     <t>Location</t>
   </si>
@@ -271,13 +272,64 @@
   </si>
   <si>
     <t>TP</t>
+  </si>
+  <si>
+    <t>to do</t>
+  </si>
+  <si>
+    <t>Fix units for P</t>
+  </si>
+  <si>
+    <t>has TDP and Sus P</t>
+  </si>
+  <si>
+    <t>no TDP or TP</t>
+  </si>
+  <si>
+    <t>as ions</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>SRP (no TDP?)</t>
+  </si>
+  <si>
+    <t>not enough data</t>
+  </si>
+  <si>
+    <t>as N</t>
+  </si>
+  <si>
+    <t>TP (david says is TDP)_</t>
+  </si>
+  <si>
+    <t>corrected</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>CAN I GET TDP HERE?</t>
+  </si>
+  <si>
+    <t>IS SO4 AS ION OR ELEMENT</t>
+  </si>
+  <si>
+    <t>DROP</t>
+  </si>
+  <si>
+    <t>We're missing DOC, does it exist?</t>
+  </si>
+  <si>
+    <t>these are FWMC - need to exclude from code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,8 +366,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +397,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -353,7 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -382,14 +447,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -707,11 +778,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72083B0E-8DDB-0E46-A41E-82CD2F50A4BE}">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L22" sqref="L22:L24"/>
+    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,7 +889,7 @@
       <c r="F3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="10" t="s">
         <v>70</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -926,18 +997,18 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="3"/>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
     </row>
     <row r="7" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1098,9 +1169,14 @@
       <c r="L10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="2"/>
+      <c r="M10" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="N10" s="2"/>
       <c r="O10" s="3"/>
+      <c r="S10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="11" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1132,6 +1208,9 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="3"/>
+      <c r="S11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1193,7 +1272,9 @@
       <c r="L13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="N13" s="2"/>
       <c r="O13" s="3"/>
     </row>
@@ -1319,7 +1400,9 @@
       <c r="L17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" s="3"/>
     </row>
@@ -1564,10 +1647,213 @@
       </c>
       <c r="O24" s="3"/>
     </row>
+    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="R6:AA6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00432CF3-689E-9141-83D3-8E8028CE9EB1}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated csv's for MARS
</commit_message>
<xml_diff>
--- a/data/JMHnewMungedDat/00_WatershedDataNotes.xlsx
+++ b/data/JMHnewMungedDat/00_WatershedDataNotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hood.211/Dropbox/JMH_dropbox/stephanson2/projects/6_Research/IrenasPaper/bgc_meta/data/JMHnewMungedDat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3C2CF2-B58F-134B-8044-BBBE5C729650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BE6A38-BC80-5D47-8E21-D8B9E1240B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{BC43E26C-2443-B84E-92D9-98FD3EC23313}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{BC43E26C-2443-B84E-92D9-98FD3EC23313}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,17 +450,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -781,15 +781,17 @@
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="C1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="14" width="23.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="7" width="23.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="14" width="23.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="34" x14ac:dyDescent="0.2">
@@ -997,18 +999,18 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="3"/>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
     </row>
     <row r="7" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1677,23 +1679,23 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14" t="s">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14" t="s">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14" t="s">
+      <c r="I28" s="12"/>
+      <c r="J28" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="K28" s="14" t="s">
+      <c r="K28" s="12" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1723,7 +1725,7 @@
       <c r="B31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="11" t="s">
         <v>87</v>
       </c>
       <c r="G31" s="1" t="s">

</xml_diff>

<commit_message>
start at LOQ analysis
</commit_message>
<xml_diff>
--- a/data/JMHnewMungedDat/00_WatershedDataNotes.xlsx
+++ b/data/JMHnewMungedDat/00_WatershedDataNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="500" windowWidth="23040" windowHeight="26380" activeTab="1"/>
+    <workbookView xWindow="25020" yWindow="0" windowWidth="25360" windowHeight="28220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="167">
   <si>
     <t>Location</t>
   </si>
@@ -325,9 +325,6 @@
     <t>Solute</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>LOQ</t>
   </si>
   <si>
@@ -337,9 +334,6 @@
     <t>Method</t>
   </si>
   <si>
-    <t>TN</t>
-  </si>
-  <si>
     <t>Date_start</t>
   </si>
   <si>
@@ -382,9 +376,6 @@
     <t>Dionex ICS1100 (Chromeleon 7 software) for all samples</t>
   </si>
   <si>
-    <t>TOC</t>
-  </si>
-  <si>
     <t>Astro Analyzer(Total Carbon) and Inorganic Carbon</t>
   </si>
   <si>
@@ -451,9 +442,6 @@
     <t>PO4</t>
   </si>
   <si>
-    <t>TKN</t>
-  </si>
-  <si>
     <t>http://andlter.forestry.oregonstate.edu/data/attributesdetail.aspx?dbcode=CF002&amp;entnum=1</t>
   </si>
   <si>
@@ -512,13 +500,46 @@
   </si>
   <si>
     <t>method detection limit</t>
+  </si>
+  <si>
+    <t>LOQ_reported</t>
+  </si>
+  <si>
+    <t>units_LOQ</t>
+  </si>
+  <si>
+    <t>Units_reported</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>LOQ sometimes defined as 10x SD, assume precision reported here = SD</t>
+  </si>
+  <si>
+    <t>mg SO4/L</t>
+  </si>
+  <si>
+    <t>as TKN</t>
+  </si>
+  <si>
+    <t>Notes_a</t>
+  </si>
+  <si>
+    <t>as TN</t>
+  </si>
+  <si>
+    <t>as TOC</t>
+  </si>
+  <si>
+    <t>as TP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -583,6 +604,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -623,7 +652,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -636,6 +665,26 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
@@ -692,7 +741,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="33">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -704,7 +753,27 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1033,7 +1102,7 @@
     <col min="8" max="14" width="23.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="34">
+    <row r="1" spans="1:27" ht="30">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1147,7 @@
       </c>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:27" ht="17">
+    <row r="2" spans="1:27">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1111,7 +1180,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="34">
+    <row r="3" spans="1:27" ht="30">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1140,7 +1209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="34">
+    <row r="4" spans="1:27" ht="30">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1177,7 +1246,7 @@
       </c>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="51">
+    <row r="5" spans="1:27" ht="45">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1208,7 +1277,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="51">
+    <row r="6" spans="1:27" ht="45">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1251,7 +1320,7 @@
       <c r="Z6" s="21"/>
       <c r="AA6" s="21"/>
     </row>
-    <row r="7" spans="1:27" ht="51">
+    <row r="7" spans="1:27" ht="45">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1312,7 +1381,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="51">
+    <row r="8" spans="1:27" ht="45">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1352,7 +1421,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:27" ht="51">
+    <row r="9" spans="1:27" ht="45">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1383,7 +1452,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="17">
+    <row r="10" spans="1:27">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1419,7 +1488,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="17">
+    <row r="11" spans="1:27">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1453,7 +1522,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="17">
+    <row r="12" spans="1:27">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1484,7 +1553,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:27" ht="17">
+    <row r="13" spans="1:27">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1519,7 +1588,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:27" ht="17">
+    <row r="14" spans="1:27">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1550,7 +1619,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:27" ht="17">
+    <row r="15" spans="1:27">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1581,7 +1650,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:27" ht="17">
+    <row r="16" spans="1:27">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1612,7 +1681,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" ht="34">
+    <row r="17" spans="1:15" ht="30">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -1647,7 +1716,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" ht="34">
+    <row r="18" spans="1:15" ht="30">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -1680,7 +1749,7 @@
       <c r="N18" s="2"/>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:15" ht="51">
+    <row r="19" spans="1:15" ht="45">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -1715,7 +1784,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="1:15" ht="51">
+    <row r="20" spans="1:15" ht="45">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -1750,7 +1819,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15" ht="68">
+    <row r="21" spans="1:15" ht="60">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1818,7 +1887,7 @@
       </c>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15" ht="136">
+    <row r="23" spans="1:15" ht="120">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
@@ -1853,7 +1922,7 @@
       </c>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="1:15" ht="136">
+    <row r="24" spans="1:15" ht="120">
       <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
@@ -1888,7 +1957,7 @@
       </c>
       <c r="O24" s="3"/>
     </row>
-    <row r="27" spans="1:15" ht="17">
+    <row r="27" spans="1:15">
       <c r="B27" s="8" t="s">
         <v>61</v>
       </c>
@@ -1917,7 +1986,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="17">
+    <row r="28" spans="1:15">
       <c r="A28" s="12"/>
       <c r="B28" s="12" t="s">
         <v>10</v>
@@ -1938,7 +2007,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="17">
+    <row r="29" spans="1:15">
       <c r="B29" s="1" t="s">
         <v>15</v>
       </c>
@@ -1949,7 +2018,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="17">
+    <row r="30" spans="1:15">
       <c r="B30" s="1" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +2029,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="34">
+    <row r="31" spans="1:15" ht="30">
       <c r="B31" s="1" t="s">
         <v>23</v>
       </c>
@@ -1980,7 +2049,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="34">
+    <row r="32" spans="1:15" ht="30">
       <c r="B32" s="1" t="s">
         <v>27</v>
       </c>
@@ -2000,7 +2069,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="34">
+    <row r="33" spans="2:11" ht="30">
       <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2014,7 +2083,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="17">
+    <row r="34" spans="2:11">
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2025,7 +2094,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="17">
+    <row r="35" spans="2:11">
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
@@ -2036,7 +2105,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="17">
+    <row r="36" spans="2:11">
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
@@ -2063,755 +2132,1057 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="17">
+    <row r="1" spans="1:13" s="14" customFormat="1" ht="30">
       <c r="A1" s="13" t="s">
         <v>61</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>96</v>
       </c>
       <c r="E1" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="17">
+        <v>42217</v>
+      </c>
+      <c r="C2" s="17">
+        <v>42339</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="H2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="K2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="17">
+        <v>42370</v>
+      </c>
+      <c r="C3" s="17">
+        <v>43370</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="F3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="H3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="K3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="17">
+        <v>36892</v>
+      </c>
+      <c r="C4" s="17">
+        <v>37653</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="H4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="17">
+        <v>36892</v>
+      </c>
+      <c r="C5" s="17">
+        <v>42216</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="F5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="H5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0.05</v>
+      </c>
+      <c r="F6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6">
+        <f>E6</f>
+        <v>0.05</v>
+      </c>
+      <c r="H6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" t="s">
+        <v>155</v>
+      </c>
+      <c r="J6" t="s">
+        <v>153</v>
+      </c>
+      <c r="K6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="17">
+        <v>34335</v>
+      </c>
+      <c r="C7" s="17">
+        <v>36526</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="16">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="16">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>0.25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8">
+        <f>E8</f>
+        <v>0.25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="K8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>0.06</v>
+      </c>
+      <c r="F9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9">
+        <f>E9*10</f>
+        <v>0.6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" t="s">
+        <v>134</v>
+      </c>
+      <c r="K9" t="s">
+        <v>136</v>
+      </c>
+      <c r="L9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="17">
+        <v>29587</v>
+      </c>
+      <c r="C10" s="17">
+        <v>33970</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="K10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="17">
+        <v>31778</v>
+      </c>
+      <c r="C11" s="17">
+        <v>35795</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11">
+        <f>E11*12*0.001</f>
+        <v>0.3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="17">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="17">
-        <v>31778</v>
-      </c>
-      <c r="C2" s="17">
-        <v>35795</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="K11" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16">
+      <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="E2">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E12">
+        <v>0.05</v>
+      </c>
+      <c r="F12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12">
+        <f>E12*10</f>
+        <v>0.5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" t="s">
         <v>134</v>
       </c>
-      <c r="G2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I2" s="18" t="s">
+      <c r="K12" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="17">
-        <v>35796</v>
-      </c>
-      <c r="C3" s="17">
-        <v>42004</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>149</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="17">
-        <v>35796</v>
-      </c>
-      <c r="C4" s="17">
-        <v>42004</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>0.5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" t="s">
-        <v>131</v>
-      </c>
-      <c r="I6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="F7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G8" t="s">
-        <v>131</v>
-      </c>
-      <c r="I8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>1.5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17">
-      <c r="A10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10">
-        <v>0.3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="I10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>0.3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="I11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="I12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="17">
+      <c r="L12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>0.02</v>
+        <v>1.5</v>
       </c>
       <c r="F13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13">
+        <f>E13</f>
+        <v>1.5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="G13" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="I13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="17">
+      <c r="K13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14">
-        <v>9.7000000000000003E-2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>151</v>
+        <v>127</v>
+      </c>
+      <c r="G14">
+        <f>E14*0.001</f>
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>103</v>
       </c>
       <c r="I14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="17">
+        <v>128</v>
+      </c>
+      <c r="K14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="B15" s="17">
+        <v>41395</v>
+      </c>
+      <c r="C15" s="17">
+        <v>43370</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="F15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>152</v>
+        <v>103</v>
+      </c>
+      <c r="G15">
+        <v>0.01</v>
+      </c>
+      <c r="H15" t="s">
+        <v>103</v>
       </c>
       <c r="I15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>102</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="K15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>0.06</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="F16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G16" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="G16">
+        <f>E16*10</f>
+        <v>0.03</v>
+      </c>
+      <c r="H16" t="s">
+        <v>138</v>
       </c>
       <c r="I16" t="s">
+        <v>134</v>
+      </c>
+      <c r="K16" t="s">
+        <v>136</v>
+      </c>
+      <c r="L16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17">
+        <f>E17</f>
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" s="19" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="17">
-      <c r="A17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>0.05</v>
-      </c>
-      <c r="F17" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17" t="s">
-        <v>137</v>
-      </c>
-      <c r="I17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="17">
+      <c r="J17" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="K17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="B18" s="17">
+        <v>29221</v>
+      </c>
+      <c r="C18" s="17">
+        <v>41334</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
-      <c r="E18">
-        <v>3.0000000000000001E-3</v>
-      </c>
       <c r="F18" t="s">
-        <v>142</v>
-      </c>
-      <c r="G18" t="s">
-        <v>137</v>
+        <v>103</v>
+      </c>
+      <c r="H18" t="s">
+        <v>103</v>
       </c>
       <c r="I18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="K18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="B19" s="17">
+        <v>35796</v>
+      </c>
+      <c r="C19" s="17">
+        <v>42004</v>
       </c>
       <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" t="s">
+        <v>145</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="E19">
-        <v>1E-3</v>
-      </c>
-      <c r="F19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" t="s">
-        <v>137</v>
-      </c>
-      <c r="I19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="17">
-      <c r="A20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
       <c r="E20">
-        <v>0.02</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G20" t="s">
-        <v>137</v>
+        <v>127</v>
+      </c>
+      <c r="G20">
+        <f>E20*0.001</f>
+        <v>1.1200000000000001E-3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>103</v>
       </c>
       <c r="I20" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="17">
+        <v>128</v>
+      </c>
+      <c r="K20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="F21" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="G21">
+        <f>E21*10</f>
+        <v>0.01</v>
+      </c>
+      <c r="H21" t="s">
+        <v>138</v>
       </c>
       <c r="I21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K21" t="s">
+        <v>136</v>
+      </c>
+      <c r="L21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="17">
+        <v>41395</v>
+      </c>
+      <c r="C22" s="17">
+        <v>43370</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>0.04</v>
+      </c>
+      <c r="F22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22">
+        <v>0.04</v>
+      </c>
+      <c r="H22" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>0.3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23">
+        <f>E23*(14/(14+16*3))</f>
+        <v>6.774193548387096E-2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I23" s="19" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="17">
-      <c r="A22" s="2" t="s">
+      <c r="J23" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="K23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="17">
+        <v>29221</v>
+      </c>
+      <c r="C24" s="17">
+        <v>34983</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="K24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="17">
+        <v>34984</v>
+      </c>
+      <c r="C25" s="17">
+        <v>41334</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" t="s">
+        <v>103</v>
+      </c>
+      <c r="I25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="K25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="17">
+        <v>35796</v>
+      </c>
+      <c r="C26" s="17">
+        <v>42004</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" t="s">
+        <v>145</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" t="s">
-        <v>138</v>
-      </c>
-      <c r="E22">
+      <c r="D27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27">
         <v>1E-3</v>
       </c>
-      <c r="F22" t="s">
-        <v>143</v>
-      </c>
-      <c r="G22" t="s">
-        <v>137</v>
-      </c>
-      <c r="I22" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="17">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="F27" t="s">
         <v>139</v>
       </c>
-      <c r="E23">
+      <c r="G27">
+        <f>E27*10</f>
         <v>0.01</v>
       </c>
-      <c r="F23" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" t="s">
-        <v>137</v>
-      </c>
-      <c r="I23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24">
-        <v>0.02</v>
-      </c>
-      <c r="F24" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" t="s">
-        <v>159</v>
-      </c>
-      <c r="H24" t="s">
-        <v>149</v>
-      </c>
-      <c r="I24" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <v>0.05</v>
-      </c>
-      <c r="F25" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" t="s">
-        <v>159</v>
-      </c>
-      <c r="H25" t="s">
-        <v>157</v>
-      </c>
-      <c r="I25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>116</v>
-      </c>
-      <c r="E26">
-        <v>0.5</v>
-      </c>
-      <c r="F26" t="s">
-        <v>105</v>
-      </c>
-      <c r="G26" t="s">
-        <v>159</v>
-      </c>
-      <c r="H26" t="s">
-        <v>158</v>
-      </c>
-      <c r="I26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="17">
-      <c r="A27" s="2" t="s">
-        <v>36</v>
+      <c r="H27" t="s">
+        <v>139</v>
       </c>
       <c r="I27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="17">
+        <v>134</v>
+      </c>
+      <c r="K27" t="s">
+        <v>136</v>
+      </c>
+      <c r="L27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="17">
-        <v>28856</v>
-      </c>
-      <c r="C28" s="15">
-        <v>34060</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="E28">
         <v>0.02</v>
       </c>
       <c r="F28" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" t="s">
-        <v>104</v>
+        <v>139</v>
+      </c>
+      <c r="G28">
+        <f>E28</f>
+        <v>0.02</v>
       </c>
       <c r="H28" t="s">
-        <v>106</v>
-      </c>
-      <c r="I28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="17">
+        <v>139</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="K28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="15">
-        <v>34090</v>
-      </c>
-      <c r="C29" s="15">
-        <v>34304</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" t="s">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>0.02</v>
+      </c>
+      <c r="F29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29">
+        <f>E29</f>
+        <v>0.02</v>
       </c>
       <c r="H29" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="I29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="17">
+        <v>155</v>
+      </c>
+      <c r="J29" t="s">
+        <v>145</v>
+      </c>
+      <c r="K29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="15">
-        <v>34335</v>
+        <v>38718</v>
       </c>
       <c r="C30" s="15">
-        <v>43344</v>
+        <v>39448</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="E30">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F30" t="s">
-        <v>105</v>
-      </c>
-      <c r="G30" t="s">
-        <v>104</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="G30">
+        <v>0.2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>103</v>
       </c>
       <c r="I30" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="K30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="15">
-        <v>29587</v>
-      </c>
-      <c r="C31" s="15">
-        <v>29983</v>
+      <c r="B31" s="17">
+        <v>39814</v>
+      </c>
+      <c r="C31" s="17">
+        <v>43370</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E31">
-        <v>1E-3</v>
+        <v>0.2</v>
       </c>
       <c r="F31" t="s">
-        <v>105</v>
-      </c>
-      <c r="G31" t="s">
-        <v>104</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>108</v>
+        <v>103</v>
+      </c>
+      <c r="G31">
+        <v>0.2</v>
+      </c>
+      <c r="H31" t="s">
+        <v>103</v>
       </c>
       <c r="I31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="K31" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="15">
-        <v>391982</v>
+        <v>29221</v>
       </c>
       <c r="C32" s="15">
-        <v>31079</v>
+        <v>30317</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E32">
-        <v>1E-3</v>
+        <v>0.5</v>
       </c>
       <c r="F32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G32" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32">
+        <v>0.5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>103</v>
+      </c>
+      <c r="I32" t="s">
+        <v>102</v>
+      </c>
+      <c r="J32" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="I32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="17">
+      <c r="K32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="15">
-        <v>31352</v>
+        <v>30682</v>
       </c>
       <c r="C33" s="15">
-        <v>43344</v>
+        <v>35065</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E33">
-        <v>1E-3</v>
+        <v>0.5</v>
       </c>
       <c r="F33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" t="s">
-        <v>104</v>
-      </c>
-      <c r="H33" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33">
+        <v>0.5</v>
+      </c>
+      <c r="H33" t="s">
+        <v>103</v>
+      </c>
+      <c r="I33" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="I33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="17">
+      <c r="K33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="15">
-        <v>29221</v>
+        <v>35431</v>
       </c>
       <c r="C34" s="15">
-        <v>30317</v>
+        <v>38353</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -2820,544 +3191,582 @@
         <v>0.5</v>
       </c>
       <c r="F34" t="s">
-        <v>105</v>
-      </c>
-      <c r="G34" t="s">
-        <v>104</v>
-      </c>
-      <c r="H34" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34">
+        <v>0.5</v>
+      </c>
+      <c r="H34" t="s">
+        <v>103</v>
+      </c>
+      <c r="I34" t="s">
+        <v>102</v>
+      </c>
+      <c r="J34" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="I34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="17">
+      <c r="K34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="15">
-        <v>30682</v>
-      </c>
-      <c r="C35" s="15">
-        <v>35065</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35">
-        <v>0.5</v>
+        <v>0.02</v>
       </c>
       <c r="F35" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" t="s">
-        <v>104</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>112</v>
+        <v>137</v>
+      </c>
+      <c r="G35">
+        <f>10*E35*((32.065+4*16))/32.065</f>
+        <v>0.59918914704506476</v>
+      </c>
+      <c r="H35" t="s">
+        <v>161</v>
       </c>
       <c r="I35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="17">
+        <v>134</v>
+      </c>
+      <c r="K35" t="s">
+        <v>136</v>
+      </c>
+      <c r="L35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="15">
-        <v>35431</v>
-      </c>
-      <c r="C36" s="15">
-        <v>38353</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
       </c>
       <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36">
+        <f>E36</f>
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>103</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="K36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37">
+        <v>0.3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>103</v>
+      </c>
+      <c r="G37">
+        <f>E37</f>
+        <v>0.3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>103</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="K37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38">
         <v>0.5</v>
       </c>
-      <c r="F36" t="s">
-        <v>105</v>
-      </c>
-      <c r="G36" t="s">
-        <v>104</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="I36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="17">
-      <c r="A37" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="15">
-        <v>38718</v>
-      </c>
-      <c r="C37" s="15">
-        <v>39448</v>
-      </c>
-      <c r="D37" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37">
-        <v>0.2</v>
-      </c>
-      <c r="F37" t="s">
-        <v>105</v>
-      </c>
-      <c r="G37" t="s">
-        <v>104</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="I37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="17">
-      <c r="A38" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="17">
-        <v>39814</v>
-      </c>
-      <c r="C38" s="17">
-        <v>43370</v>
-      </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38">
-        <v>0.2</v>
-      </c>
       <c r="F38" t="s">
-        <v>105</v>
-      </c>
-      <c r="G38" t="s">
-        <v>104</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>115</v>
+        <v>127</v>
+      </c>
+      <c r="G38">
+        <f>E38*0.001</f>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H38" t="s">
+        <v>103</v>
       </c>
       <c r="I38" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="17">
+        <v>128</v>
+      </c>
+      <c r="K38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="17">
-        <v>29952</v>
-      </c>
-      <c r="C39" s="17">
-        <v>31524</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" t="s">
-        <v>84</v>
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>2E-3</v>
       </c>
       <c r="F39" t="s">
-        <v>105</v>
-      </c>
-      <c r="G39" t="s">
-        <v>104</v>
-      </c>
-      <c r="H39" s="16" t="s">
-        <v>117</v>
+        <v>103</v>
+      </c>
+      <c r="G39">
+        <f>E39*10</f>
+        <v>0.02</v>
+      </c>
+      <c r="H39" t="s">
+        <v>103</v>
       </c>
       <c r="I39" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="17">
+        <v>134</v>
+      </c>
+      <c r="K39" t="s">
+        <v>136</v>
+      </c>
+      <c r="L39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="17">
-        <v>31525</v>
-      </c>
-      <c r="C40" s="17">
-        <v>41334</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="E40">
-        <v>0.4</v>
+        <v>0.01</v>
       </c>
       <c r="F40" t="s">
-        <v>105</v>
-      </c>
-      <c r="G40" t="s">
-        <v>104</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="G40">
+        <f>E40*10</f>
+        <v>0.1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>103</v>
       </c>
       <c r="I40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="17">
+        <v>134</v>
+      </c>
+      <c r="K40" t="s">
+        <v>136</v>
+      </c>
+      <c r="L40" t="s">
+        <v>160</v>
+      </c>
+      <c r="M40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="17">
-        <v>41395</v>
-      </c>
-      <c r="C41" s="17">
-        <v>43370</v>
+        <v>28856</v>
+      </c>
+      <c r="C41" s="15">
+        <v>34060</v>
       </c>
       <c r="D41" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="E41">
-        <v>0.4</v>
+        <v>0.02</v>
       </c>
       <c r="F41" t="s">
-        <v>105</v>
-      </c>
-      <c r="G41" t="s">
+        <v>103</v>
+      </c>
+      <c r="G41">
+        <v>0.02</v>
+      </c>
+      <c r="H41" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41" t="s">
         <v>104</v>
       </c>
-      <c r="H41" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="I41" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="17">
+      <c r="K41" t="s">
+        <v>130</v>
+      </c>
+      <c r="M41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="17">
-        <v>29221</v>
-      </c>
-      <c r="C42" s="17">
-        <v>41334</v>
+      <c r="B42" s="15">
+        <v>34335</v>
+      </c>
+      <c r="C42" s="15">
+        <v>43344</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>84</v>
+        <v>142</v>
+      </c>
+      <c r="E42">
+        <v>0.05</v>
       </c>
       <c r="F42" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42">
+        <v>0.05</v>
+      </c>
+      <c r="H42" t="s">
+        <v>103</v>
+      </c>
+      <c r="I42" t="s">
+        <v>102</v>
+      </c>
+      <c r="J42" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="G42" t="s">
-        <v>104</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="I42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="17">
+      <c r="K42" t="s">
+        <v>130</v>
+      </c>
+      <c r="M42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="17">
-        <v>41395</v>
-      </c>
-      <c r="C43" s="17">
-        <v>43370</v>
+      <c r="B43" s="15">
+        <v>34090</v>
+      </c>
+      <c r="C43" s="15">
+        <v>34304</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43">
-        <v>0.01</v>
-      </c>
-      <c r="F43" t="s">
-        <v>105</v>
-      </c>
-      <c r="G43" t="s">
-        <v>104</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="I43" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="17">
+        <v>142</v>
+      </c>
+      <c r="J43" t="s">
+        <v>84</v>
+      </c>
+      <c r="K43" t="s">
+        <v>130</v>
+      </c>
+      <c r="M43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="17">
-        <v>29221</v>
+        <v>31525</v>
       </c>
       <c r="C44" s="17">
-        <v>34983</v>
+        <v>41334</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" t="s">
-        <v>84</v>
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>0.4</v>
       </c>
       <c r="F44" t="s">
-        <v>105</v>
-      </c>
-      <c r="G44" t="s">
-        <v>104</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>122</v>
+        <v>103</v>
+      </c>
+      <c r="G44">
+        <v>0.4</v>
+      </c>
+      <c r="H44" t="s">
+        <v>103</v>
       </c>
       <c r="I44" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="K44" t="s">
+        <v>130</v>
+      </c>
+      <c r="M44" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="17">
-        <v>34984</v>
+        <v>41395</v>
       </c>
       <c r="C45" s="17">
-        <v>41334</v>
+        <v>43370</v>
       </c>
       <c r="D45" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" t="s">
-        <v>84</v>
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>0.4</v>
       </c>
       <c r="F45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G45" t="s">
-        <v>104</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>123</v>
+        <v>103</v>
+      </c>
+      <c r="G45">
+        <v>0.4</v>
+      </c>
+      <c r="H45" t="s">
+        <v>103</v>
       </c>
       <c r="I45" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="K45" t="s">
+        <v>130</v>
+      </c>
+      <c r="M45" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="17">
-        <v>41395</v>
-      </c>
-      <c r="C46" s="17">
-        <v>43370</v>
+        <v>33</v>
       </c>
       <c r="D46" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E46">
-        <v>0.04</v>
+        <v>0.5</v>
       </c>
       <c r="F46" t="s">
-        <v>105</v>
-      </c>
-      <c r="G46" t="s">
-        <v>104</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>121</v>
+        <v>103</v>
+      </c>
+      <c r="G46">
+        <f>E46</f>
+        <v>0.5</v>
+      </c>
+      <c r="H46" t="s">
+        <v>103</v>
       </c>
       <c r="I46" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="17">
+        <v>155</v>
+      </c>
+      <c r="J46" t="s">
+        <v>154</v>
+      </c>
+      <c r="K46" t="s">
+        <v>152</v>
+      </c>
+      <c r="M46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B47" s="17">
-        <v>29587</v>
+        <v>29952</v>
       </c>
       <c r="C47" s="17">
-        <v>33970</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>84</v>
+        <v>31524</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>105</v>
-      </c>
-      <c r="G47" t="s">
-        <v>104</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>124</v>
+        <v>103</v>
+      </c>
+      <c r="H47" t="s">
+        <v>103</v>
       </c>
       <c r="I47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="K47" t="s">
+        <v>130</v>
+      </c>
+      <c r="M47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="17">
-        <v>34335</v>
-      </c>
-      <c r="C48" s="17">
-        <v>36526</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="16">
-        <v>7.4999999999999997E-2</v>
+      <c r="B48" s="15">
+        <v>29587</v>
+      </c>
+      <c r="C48" s="15">
+        <v>29983</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48">
+        <v>1E-3</v>
       </c>
       <c r="F48" t="s">
-        <v>105</v>
-      </c>
-      <c r="G48" t="s">
-        <v>104</v>
-      </c>
-      <c r="H48" s="16" t="s">
-        <v>125</v>
+        <v>103</v>
+      </c>
+      <c r="G48">
+        <v>1E-3</v>
+      </c>
+      <c r="H48" t="s">
+        <v>103</v>
       </c>
       <c r="I48" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="K48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="17">
-        <v>36892</v>
-      </c>
-      <c r="C49" s="17">
-        <v>37653</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="16">
-        <v>0.02</v>
+      <c r="B49" s="15">
+        <v>391982</v>
+      </c>
+      <c r="C49" s="15">
+        <v>31079</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <v>1E-3</v>
       </c>
       <c r="F49" t="s">
-        <v>105</v>
-      </c>
-      <c r="G49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H49" s="16" t="s">
-        <v>126</v>
+        <v>103</v>
+      </c>
+      <c r="G49">
+        <v>1E-3</v>
+      </c>
+      <c r="H49" t="s">
+        <v>103</v>
       </c>
       <c r="I49" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M49" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="17">
-        <v>36892</v>
-      </c>
-      <c r="C50" s="17">
-        <v>42216</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" s="16">
-        <v>0.02</v>
+      <c r="B50" s="15">
+        <v>31352</v>
+      </c>
+      <c r="C50" s="15">
+        <v>43344</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>1E-3</v>
       </c>
       <c r="F50" t="s">
-        <v>105</v>
-      </c>
-      <c r="G50" t="s">
-        <v>104</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>127</v>
+        <v>103</v>
+      </c>
+      <c r="G50">
+        <v>1E-3</v>
+      </c>
+      <c r="H50" t="s">
+        <v>103</v>
       </c>
       <c r="I50" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="17">
+        <v>102</v>
+      </c>
+      <c r="J50" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="K50" t="s">
+        <v>130</v>
+      </c>
+      <c r="M50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B51" s="17">
-        <v>42217</v>
-      </c>
-      <c r="C51" s="17">
-        <v>42339</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F51" t="s">
-        <v>105</v>
-      </c>
-      <c r="G51" t="s">
-        <v>104</v>
-      </c>
-      <c r="H51" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="I51" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="17">
+        <v>17</v>
+      </c>
+      <c r="K51" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" s="17">
-        <v>42370</v>
-      </c>
-      <c r="C52" s="17">
-        <v>43370</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E52" s="16">
-        <v>0.01</v>
-      </c>
-      <c r="F52" t="s">
-        <v>105</v>
-      </c>
-      <c r="G52" t="s">
-        <v>104</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="I52" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>36</v>
+      </c>
+      <c r="K52" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="D53" s="16"/>
     </row>
   </sheetData>
+  <sortState ref="A2:L53">
+    <sortCondition ref="D2:D53"/>
+    <sortCondition ref="G2:G53"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Now uses most recent data from US data providers. Data goes from 1985 to most recent available to us.
</commit_message>
<xml_diff>
--- a/data/JMHnewMungedDat/00_WatershedDataNotes.xlsx
+++ b/data/JMHnewMungedDat/00_WatershedDataNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hood.211/Dropbox/JMH_dropbox/stephanson2/projects/6_Research/IrenasPaper/bgc_meta/data/JMHnewMungedDat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BE6A38-BC80-5D47-8E21-D8B9E1240B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE747CA8-C5A0-D749-A257-D495814F0DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{BC43E26C-2443-B84E-92D9-98FD3EC23313}"/>
+    <workbookView xWindow="51200" yWindow="1000" windowWidth="51200" windowHeight="28340" xr2:uid="{BC43E26C-2443-B84E-92D9-98FD3EC23313}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="97">
   <si>
     <t>Location</t>
   </si>
@@ -319,10 +319,13 @@
     <t>DROP</t>
   </si>
   <si>
-    <t>We're missing DOC, does it exist?</t>
-  </si>
-  <si>
     <t>these are FWMC - need to exclude from code</t>
+  </si>
+  <si>
+    <t>DROPPED [TP (david says is TDP)]</t>
+  </si>
+  <si>
+    <t>DROPPED</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -461,6 +464,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -778,20 +784,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72083B0E-8DDB-0E46-A41E-82CD2F50A4BE}">
-  <dimension ref="A1:AA36"/>
+  <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="C1:G1048576"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="7" width="23.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="14" width="23.33203125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="10.33203125" style="1" customWidth="1"/>
+    <col min="5" max="14" width="23.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="34" x14ac:dyDescent="0.2">
@@ -1741,12 +1745,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>83</v>
@@ -1772,15 +1773,21 @@
         <v>90</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="34" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>88</v>
+      <c r="F34" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>90</v>
@@ -1806,6 +1813,12 @@
       </c>
       <c r="J36" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C38" s="1">
+        <f>10^1.5</f>
+        <v>31.622776601683803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>